<commit_message>
Adding latest purchase from amplifiedparts.com
</commit_message>
<xml_diff>
--- a/BOM/amplifiedparts-dot-com BOM.xlsx
+++ b/BOM/amplifiedparts-dot-com BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ryan/Documents/GitHub/steel-string-singer-sn-002/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E0FC59E-5195-B148-A862-ECAE9DBFD02C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53509C90-FC8C-6A48-A923-A333D6084A49}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="3560" windowWidth="30880" windowHeight="16940" xr2:uid="{0199555C-9F6B-9B4E-9B9C-1898FA1D406E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="138">
   <si>
     <t>Qty Ordered</t>
   </si>
@@ -361,6 +361,90 @@
   </si>
   <si>
     <t>amplifiedparts.com</t>
+  </si>
+  <si>
+    <t>C-PD001-600</t>
+  </si>
+  <si>
+    <t>Capacitor - 600V, 716P Series, Polypropylene, Capacitance: .001 uF</t>
+  </si>
+  <si>
+    <t>C-LD022-630</t>
+  </si>
+  <si>
+    <t>Capacitor - 630V, Polypropylene, radial leads, Capacitance: .022 uF</t>
+  </si>
+  <si>
+    <t>R-B33K</t>
+  </si>
+  <si>
+    <t>Resistors - 1W, Carbon Film, Resistance: 33 kOhm</t>
+  </si>
+  <si>
+    <t>P-H1590B</t>
+  </si>
+  <si>
+    <t>Chassis Box - Hammond, Unpainted Aluminum, 4.37" x 2.37" x 1.22"</t>
+  </si>
+  <si>
+    <t>P-K302</t>
+  </si>
+  <si>
+    <t>Knob - Chicken Head, Raised, Color: Black</t>
+  </si>
+  <si>
+    <t>C-LD001-630</t>
+  </si>
+  <si>
+    <t>Capacitor - 630V, Polypropylene, radial leads, Capacitance: .001 uF</t>
+  </si>
+  <si>
+    <t>S-HLW6</t>
+  </si>
+  <si>
+    <t>Washer - Internal Tooth Lock, Zinc, Size: #6</t>
+  </si>
+  <si>
+    <t>P-H395</t>
+  </si>
+  <si>
+    <t>Switch - Rotary, 3 Poles, 3 Position</t>
+  </si>
+  <si>
+    <t>S-HLW38</t>
+  </si>
+  <si>
+    <t>Washer - Internal Tooth Lock, Zinc, Size: 3/8"</t>
+  </si>
+  <si>
+    <t>S-H173</t>
+  </si>
+  <si>
+    <t>Standoff - #6-32, Female, Aluminum, Length: 3/4"</t>
+  </si>
+  <si>
+    <t>S-H172</t>
+  </si>
+  <si>
+    <t>Standoff - #6-32, Female, Aluminum, Length: 1/2"</t>
+  </si>
+  <si>
+    <t>T-5751-PS-TAD</t>
+  </si>
+  <si>
+    <t>Vacuum Tube - 5751, Tube Amp Doctor, Premium Selected</t>
+  </si>
+  <si>
+    <t>T-7025-HG-TAD</t>
+  </si>
+  <si>
+    <t>Vacuum Tube - 7025, Tube Amp Doctor, High Grade</t>
+  </si>
+  <si>
+    <t>T-6L6WGC-TAD-MQ</t>
+  </si>
+  <si>
+    <t>Vacuum Tube - 6L6WGC, Tube Amp Doctor, Single or Matched: Matched Quad</t>
   </si>
 </sst>
 </file>
@@ -751,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBE67D0-6312-A44B-85E3-458F1293B8D9}">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1919,6 +2003,351 @@
       </c>
       <c r="G52" s="4">
         <v>3.82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>1</v>
+      </c>
+      <c r="B53" s="2">
+        <v>1</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F53" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G53" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>1</v>
+      </c>
+      <c r="B54" s="2">
+        <v>1</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F54" s="4">
+        <v>0.36</v>
+      </c>
+      <c r="G54" s="4">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>5</v>
+      </c>
+      <c r="B55" s="2">
+        <v>5</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F55" s="4">
+        <v>2</v>
+      </c>
+      <c r="G55" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>1</v>
+      </c>
+      <c r="B56" s="2">
+        <v>1</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F56" s="4">
+        <v>7.07</v>
+      </c>
+      <c r="G56" s="4">
+        <v>7.07</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>2</v>
+      </c>
+      <c r="B57" s="2">
+        <v>2</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F57" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="G57" s="4">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
+        <v>2</v>
+      </c>
+      <c r="B58" s="2">
+        <v>2</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F58" s="4">
+        <v>0.34</v>
+      </c>
+      <c r="G58" s="4">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>25</v>
+      </c>
+      <c r="B59" s="2">
+        <v>25</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F59" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="G59" s="4">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>2</v>
+      </c>
+      <c r="B60" s="2">
+        <v>2</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F60" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="G60" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A61" s="2">
+        <v>15</v>
+      </c>
+      <c r="B61" s="2">
+        <v>15</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F61" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="G61" s="4">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
+        <v>25</v>
+      </c>
+      <c r="B62" s="2">
+        <v>25</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F62" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="G62" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A63" s="2">
+        <v>20</v>
+      </c>
+      <c r="B63" s="2">
+        <v>20</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F63" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G63" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" s="2">
+        <v>20</v>
+      </c>
+      <c r="B64" s="2">
+        <v>20</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F64" s="4">
+        <v>2</v>
+      </c>
+      <c r="G64" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A65" s="2">
+        <v>1</v>
+      </c>
+      <c r="B65" s="2">
+        <v>1</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F65" s="4">
+        <v>18.95</v>
+      </c>
+      <c r="G65" s="4">
+        <v>18.95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A66" s="2">
+        <v>6</v>
+      </c>
+      <c r="B66" s="2">
+        <v>6</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F66" s="4">
+        <v>19.95</v>
+      </c>
+      <c r="G66" s="4">
+        <v>119.7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A67" s="2">
+        <v>1</v>
+      </c>
+      <c r="B67" s="2">
+        <v>1</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F67" s="4">
+        <v>98</v>
+      </c>
+      <c r="G67" s="4">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1972,6 +2401,21 @@
     <hyperlink ref="D50" r:id="rId47" display="https://www.amplifiedparts.com/products/screw-632-phillips-pan-head-machine-zinc" xr:uid="{3ECEA5B5-DB19-BB4F-AC85-C6C9A79966C1}"/>
     <hyperlink ref="D51" r:id="rId48" display="https://www.amplifiedparts.com/products/standoff-6-32-male-female-aluminum" xr:uid="{F6EFB850-444B-0742-A34A-6265D06CAA71}"/>
     <hyperlink ref="D52" r:id="rId49" display="https://www.amplifiedparts.com/products/standoff-6-32-male-female-aluminum" xr:uid="{93CE6923-C9BB-174B-97A9-6CC6F2371780}"/>
+    <hyperlink ref="D53" r:id="rId50" display="https://www.amplifiedparts.com/products/capacitor-600v-716p-series-polypropylene" xr:uid="{01626727-D59A-AE45-904D-5DEC75010C93}"/>
+    <hyperlink ref="D54" r:id="rId51" display="https://www.amplifiedparts.com/products/capacitor-630v-polypropylene-radial-leads" xr:uid="{4EBB18AD-6100-884D-9D78-7A16607C118D}"/>
+    <hyperlink ref="D55" r:id="rId52" display="https://www.amplifiedparts.com/products/resistors-1w-carbon-film" xr:uid="{97E71238-E0D9-ED41-9FD4-55881FCCF1AE}"/>
+    <hyperlink ref="D56" r:id="rId53" display="https://www.amplifiedparts.com/products/chassis-box-hammond-unpainted-aluminum-437-x-237-x-122" xr:uid="{31888DCA-4426-444B-974A-E6526716EDE8}"/>
+    <hyperlink ref="D57" r:id="rId54" display="https://www.amplifiedparts.com/products/knob-chicken-head-raised" xr:uid="{B52594DC-6909-744D-BA87-2F3FD68B4AB0}"/>
+    <hyperlink ref="D58" r:id="rId55" display="https://www.amplifiedparts.com/products/capacitor-630v-polypropylene-radial-leads" xr:uid="{380C44B3-A3EB-2749-A694-BF348911BD2C}"/>
+    <hyperlink ref="D59" r:id="rId56" display="https://www.amplifiedparts.com/products/washer-internal-tooth-lock-zinc" xr:uid="{CB280860-5B31-6B41-8429-926A58467AD1}"/>
+    <hyperlink ref="D60" r:id="rId57" display="https://www.amplifiedparts.com/products/switch-rotary-3-poles-3-position" xr:uid="{5B95EB76-4FF1-6441-A991-5F4A5418B58E}"/>
+    <hyperlink ref="D61" r:id="rId58" display="https://www.amplifiedparts.com/products/washer-internal-tooth-lock-zinc" xr:uid="{44407C4A-3B71-0842-826A-41E11485AA86}"/>
+    <hyperlink ref="D62" r:id="rId59" display="https://www.amplifiedparts.com/products/screw-632-phillips-pan-head-machine-zinc" xr:uid="{73EDBF5B-1C0A-4242-A457-D205A55272C8}"/>
+    <hyperlink ref="D63" r:id="rId60" display="https://www.amplifiedparts.com/products/standoff-6-32-female-aluminum" xr:uid="{7F61D612-6EC6-D949-8C75-E83B72324ABA}"/>
+    <hyperlink ref="D64" r:id="rId61" display="https://www.amplifiedparts.com/products/standoff-6-32-female-aluminum" xr:uid="{EC4736A9-C917-C843-AF22-752E5FEB23DC}"/>
+    <hyperlink ref="D65" r:id="rId62" display="https://www.amplifiedparts.com/products/vacuum-tube-5751-tube-amp-doctor-premium-selected" xr:uid="{4912950B-C7F1-1948-82EA-45DE26B3F712}"/>
+    <hyperlink ref="D66" r:id="rId63" display="https://www.amplifiedparts.com/products/vacuum-tube-7025-tube-amp-doctor-high-grade" xr:uid="{9BD8E76F-19D2-3843-B818-7B8EB02F1E31}"/>
+    <hyperlink ref="D67" r:id="rId64" display="https://www.amplifiedparts.com/products/vacuum-tube-6l6wgc-tube-amp-doctor" xr:uid="{98CAA186-DA25-FC44-820D-1F20A7DE47BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added correct part number for ClassicTone OT with standoff
</commit_message>
<xml_diff>
--- a/BOM/amplifiedparts-dot-com BOM.xlsx
+++ b/BOM/amplifiedparts-dot-com BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ryan/Documents/GitHub/steel-string-singer-sn-002/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CD3F6D-C499-4146-8191-9DD3AADB1B49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A787E121-BF61-E743-A095-84844123CDC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{0199555C-9F6B-9B4E-9B9C-1898FA1D406E}"/>
   </bookViews>
@@ -832,7 +832,7 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D23" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fixed an error with output transformer selection
</commit_message>
<xml_diff>
--- a/BOM/amplifiedparts-dot-com BOM.xlsx
+++ b/BOM/amplifiedparts-dot-com BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ryan/Documents/GitHub/steel-string-singer-sn-002/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A787E121-BF61-E743-A095-84844123CDC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC2048F-FE27-544B-9FE5-F7BC9DD60950}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{0199555C-9F6B-9B4E-9B9C-1898FA1D406E}"/>
   </bookViews>
@@ -425,7 +425,7 @@
     <t>1/4" Jack - Switchcraft, Mono, open circuit, Bushing Length: Standard (0.275")</t>
   </si>
   <si>
-    <t>Alternative to ClassicTone 40-18012</t>
+    <t>Alternative to ClassicTone 40-18102</t>
   </si>
 </sst>
 </file>
@@ -832,7 +832,7 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D23" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add some useful items and visuals to Boms
Updated 4-40 quantities to match needs
Add Solder Washer Lugs
Correct Fuse IDs
</commit_message>
<xml_diff>
--- a/BOM/amplifiedparts-dot-com BOM.xlsx
+++ b/BOM/amplifiedparts-dot-com BOM.xlsx
@@ -1,32 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ryan/Documents/GitHub/steel-string-singer-sn-002/BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WesMi\Documents\Music Equipment\steel-string-singer-sn-002\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC2048F-FE27-544B-9FE5-F7BC9DD60950}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4F6ADF-3132-44FF-B564-68C26411DC15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{0199555C-9F6B-9B4E-9B9C-1898FA1D406E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0199555C-9F6B-9B4E-9B9C-1898FA1D406E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -77,15 +69,9 @@
     <t>Fuse Holder - 3AG-Type, High Quality</t>
   </si>
   <si>
-    <t>F-ZS010</t>
-  </si>
-  <si>
     <t>Fuse - Slow-Blow, 250V, 3AG, 0.25" x 1.25", Amperage: 1 Amps</t>
   </si>
   <si>
-    <t>F-ZS035</t>
-  </si>
-  <si>
     <t>Fuse - Slow-Blow, 250V, 3AG, 0.25" x 1.25", Amperage: 4 Amps</t>
   </si>
   <si>
@@ -332,9 +318,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>For the Smooth &amp; Slim clone</t>
-  </si>
-  <si>
     <t>Reverb &amp; V1 option</t>
   </si>
   <si>
@@ -426,6 +409,27 @@
   </si>
   <si>
     <t>Alternative to ClassicTone 40-18102</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For the Smooth &amp; Slim clone </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Not for SSS #002)</t>
+    </r>
+  </si>
+  <si>
+    <t>F-Z3AG-S1</t>
+  </si>
+  <si>
+    <t>F-Z3AG-S4</t>
   </si>
 </sst>
 </file>
@@ -435,7 +439,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -480,13 +484,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -502,7 +519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -514,6 +531,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -831,29 +852,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBE67D0-6312-A44B-85E3-458F1293B8D9}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D23" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="97.6640625" customWidth="1"/>
-    <col min="5" max="5" width="29.1640625" customWidth="1"/>
-    <col min="6" max="6" width="38.33203125" customWidth="1"/>
+    <col min="4" max="4" width="97.625" customWidth="1"/>
+    <col min="5" max="5" width="29.125" customWidth="1"/>
+    <col min="6" max="6" width="38.375" customWidth="1"/>
     <col min="7" max="7" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="5" customFormat="1" ht="31.5">
       <c r="A1" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18">
       <c r="A3" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -865,16 +886,16 @@
         <v>2</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -895,9 +916,9 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="18">
       <c r="A5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -913,12 +934,12 @@
       </c>
       <c r="F5" s="4">
         <f t="shared" ref="F5:F57" si="0">A5*E5</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18">
       <c r="A6" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -934,10 +955,10 @@
       </c>
       <c r="F6" s="4">
         <f t="shared" si="0"/>
-        <v>0.31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -958,7 +979,7 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="18">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -966,10 +987,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="E8" s="4">
         <v>2.93</v>
@@ -979,7 +1000,7 @@
         <v>5.86</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="18">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -987,10 +1008,10 @@
         <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>16</v>
+        <v>130</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="4">
         <v>2.93</v>
@@ -1000,7 +1021,7 @@
         <v>5.86</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="18">
       <c r="A10" s="2">
         <v>5</v>
       </c>
@@ -1008,10 +1029,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E10" s="4">
         <v>0.9</v>
@@ -1021,7 +1042,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="18">
       <c r="A11" s="2">
         <v>2</v>
       </c>
@@ -1029,10 +1050,10 @@
         <v>3</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E11" s="4">
         <v>1.44</v>
@@ -1042,7 +1063,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="18">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -1050,10 +1071,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E12" s="4">
         <v>1.44</v>
@@ -1063,7 +1084,7 @@
         <v>4.32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="18">
       <c r="A13" s="2">
         <v>2</v>
       </c>
@@ -1071,10 +1092,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E13" s="4">
         <v>1.44</v>
@@ -1084,7 +1105,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="18">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -1092,10 +1113,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E14" s="4">
         <v>1.76</v>
@@ -1105,7 +1126,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="18">
       <c r="A15" s="2">
         <v>1</v>
       </c>
@@ -1113,10 +1134,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E15" s="4">
         <v>3.15</v>
@@ -1126,7 +1147,7 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="18">
       <c r="A16" s="2">
         <v>1</v>
       </c>
@@ -1134,10 +1155,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E16" s="4">
         <v>0.41</v>
@@ -1147,10 +1168,10 @@
         <v>0.41</v>
       </c>
       <c r="G16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18">
       <c r="A17" s="2">
         <v>7</v>
       </c>
@@ -1158,10 +1179,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E17" s="4">
         <v>1.22</v>
@@ -1171,7 +1192,7 @@
         <v>8.5399999999999991</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="18">
       <c r="A18" s="2">
         <v>3</v>
       </c>
@@ -1179,10 +1200,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E18" s="4">
         <v>0.86</v>
@@ -1192,7 +1213,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="18">
       <c r="A19" s="2">
         <v>3</v>
       </c>
@@ -1200,10 +1221,10 @@
         <v>3</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E19" s="4">
         <v>0.86</v>
@@ -1213,7 +1234,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="18">
       <c r="A20" s="2">
         <v>6</v>
       </c>
@@ -1221,10 +1242,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E20" s="4">
         <v>1.35</v>
@@ -1234,7 +1255,7 @@
         <v>8.1000000000000014</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="18">
       <c r="A21" s="2">
         <v>2</v>
       </c>
@@ -1242,10 +1263,10 @@
         <v>3</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E21" s="4">
         <v>1.65</v>
@@ -1255,7 +1276,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="18">
       <c r="A22" s="2">
         <v>1</v>
       </c>
@@ -1263,10 +1284,10 @@
         <v>3</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E22" s="4">
         <v>0.77</v>
@@ -1276,7 +1297,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="18">
       <c r="A23" s="2">
         <v>1</v>
       </c>
@@ -1284,10 +1305,10 @@
         <v>3</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E23" s="4">
         <v>3.55</v>
@@ -1297,10 +1318,10 @@
         <v>3.55</v>
       </c>
       <c r="G23" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="18">
       <c r="A24" s="2">
         <v>2</v>
       </c>
@@ -1308,10 +1329,10 @@
         <v>3</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E24" s="4">
         <v>6.26</v>
@@ -1321,7 +1342,7 @@
         <v>12.52</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="18">
       <c r="A25" s="2">
         <v>2</v>
       </c>
@@ -1329,10 +1350,10 @@
         <v>3</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E25" s="4">
         <v>6.75</v>
@@ -1342,7 +1363,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="18">
       <c r="A26" s="2">
         <v>3</v>
       </c>
@@ -1350,10 +1371,10 @@
         <v>3</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E26" s="4">
         <v>3.55</v>
@@ -1363,7 +1384,7 @@
         <v>10.649999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="18">
       <c r="A27" s="2">
         <v>1</v>
       </c>
@@ -1371,10 +1392,10 @@
         <v>3</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E27" s="4">
         <v>20.66</v>
@@ -1384,7 +1405,7 @@
         <v>20.66</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="18">
       <c r="A28" s="2">
         <v>4</v>
       </c>
@@ -1392,10 +1413,10 @@
         <v>3</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E28" s="4">
         <v>3.15</v>
@@ -1405,7 +1426,7 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="18">
       <c r="A29" s="2">
         <v>2</v>
       </c>
@@ -1413,10 +1434,10 @@
         <v>3</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E29" s="4">
         <v>3.56</v>
@@ -1426,7 +1447,7 @@
         <v>7.12</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="18">
       <c r="A30" s="2">
         <v>3</v>
       </c>
@@ -1434,10 +1455,10 @@
         <v>3</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E30" s="4">
         <v>4.2</v>
@@ -1447,10 +1468,10 @@
         <v>12.600000000000001</v>
       </c>
       <c r="G30" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="18">
       <c r="A31" s="2">
         <v>2</v>
       </c>
@@ -1458,10 +1479,10 @@
         <v>3</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E31" s="4">
         <v>2.0299999999999998</v>
@@ -1471,7 +1492,7 @@
         <v>4.0599999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="18">
       <c r="A32" s="2">
         <v>4</v>
       </c>
@@ -1479,10 +1500,10 @@
         <v>3</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E32" s="4">
         <v>1.57</v>
@@ -1492,7 +1513,7 @@
         <v>6.28</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="18">
       <c r="A33" s="2">
         <v>2</v>
       </c>
@@ -1500,10 +1521,10 @@
         <v>3</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E33" s="4">
         <v>2.0699999999999998</v>
@@ -1513,7 +1534,7 @@
         <v>4.1399999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="18">
       <c r="A34" s="2">
         <v>1</v>
       </c>
@@ -1521,10 +1542,10 @@
         <v>3</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E34" s="4">
         <v>33.03</v>
@@ -1534,7 +1555,7 @@
         <v>33.03</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="18">
       <c r="A35" s="2">
         <v>3</v>
       </c>
@@ -1542,10 +1563,10 @@
         <v>6</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E35" s="4">
         <v>0.9</v>
@@ -1555,7 +1576,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="18">
       <c r="A36" s="2">
         <v>10</v>
       </c>
@@ -1563,10 +1584,10 @@
         <v>9</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E36" s="4">
         <v>0.36</v>
@@ -1576,7 +1597,7 @@
         <v>3.5999999999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="18">
       <c r="A37" s="2">
         <v>10</v>
       </c>
@@ -1584,10 +1605,10 @@
         <v>9</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E37" s="4">
         <v>0.36</v>
@@ -1597,223 +1618,223 @@
         <v>3.5999999999999996</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
+    <row r="38" spans="1:7" ht="18">
+      <c r="A38" s="10">
         <v>2</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E38" s="4">
+      <c r="B38" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E38" s="11">
         <v>1.94</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="11">
         <f>A38*E38</f>
         <v>3.88</v>
       </c>
-      <c r="G38" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
+      <c r="G38" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="18">
+      <c r="A39" s="10">
         <v>1</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="B39" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E39" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F39" s="11">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="18">
+      <c r="A40" s="10">
+        <v>1</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D40" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E39" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F39" s="4">
-        <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G39" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
+      <c r="E40" s="11">
+        <v>0.36</v>
+      </c>
+      <c r="F40" s="11">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="18">
+      <c r="A41" s="10">
         <v>1</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40" s="3" t="s">
+      <c r="B41" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D41" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E40" s="4">
-        <v>0.36</v>
-      </c>
-      <c r="F40" s="4">
-        <f t="shared" si="0"/>
-        <v>0.36</v>
-      </c>
-      <c r="G40" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
+      <c r="E41" s="11">
+        <v>2</v>
+      </c>
+      <c r="F41" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="18">
+      <c r="A42" s="10">
         <v>1</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C42" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E42" s="11">
+        <v>2</v>
+      </c>
+      <c r="F42" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="18">
+      <c r="A43" s="10">
+        <v>1</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D43" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E43" s="11">
+        <v>7.07</v>
+      </c>
+      <c r="F43" s="11">
+        <f t="shared" si="0"/>
+        <v>7.07</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="18">
+      <c r="A44" s="10">
         <v>2</v>
       </c>
-      <c r="F41" s="4">
-        <f t="shared" si="0"/>
+      <c r="B44" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E44" s="11">
+        <v>1.4</v>
+      </c>
+      <c r="F44" s="11">
+        <f t="shared" si="0"/>
+        <v>2.8</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="18">
+      <c r="A45" s="10">
+        <v>1</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E45" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="F45" s="11">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="18">
+      <c r="A46" s="10">
         <v>2</v>
       </c>
-      <c r="G41" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
-        <v>1</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E42" s="4">
-        <v>2</v>
-      </c>
-      <c r="F42" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G42" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A43" s="2">
-        <v>1</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E43" s="4">
-        <v>7.07</v>
-      </c>
-      <c r="F43" s="4">
-        <f t="shared" si="0"/>
-        <v>7.07</v>
-      </c>
-      <c r="G43" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A44" s="2">
-        <v>2</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" s="3" t="s">
+      <c r="B46" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D46" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E44" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="F44" s="4">
-        <f t="shared" si="0"/>
-        <v>2.8</v>
-      </c>
-      <c r="G44" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A45" s="2">
-        <v>1</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E45" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="F45" s="4">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="G45" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A46" s="2">
-        <v>2</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E46" s="4">
+      <c r="E46" s="11">
         <v>0.34</v>
       </c>
-      <c r="F46" s="4">
+      <c r="F46" s="11">
         <f t="shared" si="0"/>
         <v>0.68</v>
       </c>
-      <c r="G46" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="G46" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="18">
       <c r="A47" s="2">
         <v>10</v>
       </c>
@@ -1821,10 +1842,10 @@
         <v>9</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E47" s="4">
         <v>0.45</v>
@@ -1834,31 +1855,31 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
+    <row r="48" spans="1:7" ht="18">
+      <c r="A48" s="10">
         <v>1</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E48" s="4">
+      <c r="B48" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E48" s="11">
         <v>2.5</v>
       </c>
-      <c r="F48" s="4">
+      <c r="F48" s="11">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G48" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="G48" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="18">
       <c r="A49" s="2">
         <v>2</v>
       </c>
@@ -1866,10 +1887,10 @@
         <v>9</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E49" s="4">
         <v>0.65</v>
@@ -1879,18 +1900,18 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="18">
       <c r="A50" s="2">
         <v>5</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E50" s="4">
         <v>2</v>
@@ -1900,7 +1921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="18">
       <c r="A51" s="2">
         <v>1</v>
       </c>
@@ -1908,10 +1929,10 @@
         <v>3</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E51" s="4">
         <v>94.78</v>
@@ -1921,10 +1942,10 @@
         <v>94.78</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="18">
       <c r="A52" s="2">
         <v>1</v>
       </c>
@@ -1932,10 +1953,10 @@
         <v>3</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E52" s="4">
         <v>18.95</v>
@@ -1945,10 +1966,10 @@
         <v>18.95</v>
       </c>
       <c r="G52" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="18">
       <c r="A53" s="2">
         <v>1</v>
       </c>
@@ -1956,10 +1977,10 @@
         <v>3</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E53" s="4">
         <v>17.86</v>
@@ -1969,10 +1990,10 @@
         <v>17.86</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="18">
       <c r="A54" s="2">
         <v>1</v>
       </c>
@@ -1980,10 +2001,10 @@
         <v>3</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E54" s="4">
         <v>113.86</v>
@@ -1993,10 +2014,10 @@
         <v>113.86</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="18">
       <c r="A55" s="2">
         <v>2</v>
       </c>
@@ -2004,10 +2025,10 @@
         <v>3</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E55" s="4">
         <v>18.95</v>
@@ -2017,10 +2038,10 @@
         <v>37.9</v>
       </c>
       <c r="G55" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="18">
       <c r="A56" s="2">
         <v>6</v>
       </c>
@@ -2028,10 +2049,10 @@
         <v>3</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E56" s="4">
         <v>19.95</v>
@@ -2041,10 +2062,10 @@
         <v>119.69999999999999</v>
       </c>
       <c r="G56" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="18">
       <c r="A57" s="2">
         <v>1</v>
       </c>
@@ -2052,10 +2073,10 @@
         <v>3</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E57" s="4">
         <v>98</v>
@@ -2065,13 +2086,13 @@
         <v>98</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7">
       <c r="E60" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F60" s="7">
         <f>SUM(F4:F57)</f>
-        <v>754.47</v>
+        <v>756.3</v>
       </c>
     </row>
   </sheetData>
@@ -2079,59 +2100,59 @@
     <hyperlink ref="C4" r:id="rId1" display="https://www.amplifiedparts.com/products/tip-jack-insulated-deluxe" xr:uid="{B50FA0ED-DA37-B94B-8FB7-BC2680DD41DA}"/>
     <hyperlink ref="C5" r:id="rId2" display="https://www.amplifiedparts.com/products/nut-kep-zinc-package-10" xr:uid="{CCBD8C90-25E6-7C40-AA93-0F2D9A910470}"/>
     <hyperlink ref="C6" r:id="rId3" display="https://www.amplifiedparts.com/products/screw-440-phillips-pan-head-machine" xr:uid="{F970D1F6-0595-8A43-A17E-86482982293C}"/>
-    <hyperlink ref="C8" r:id="rId4" display="https://www.amplifiedparts.com/products/fuse-slo-blo-025-x-125" xr:uid="{CB55DA37-E898-DD4C-A111-82ED00860EB5}"/>
-    <hyperlink ref="C9" r:id="rId5" display="https://www.amplifiedparts.com/products/fuse-slo-blo-025-x-125" xr:uid="{62FD5CAC-91EB-0341-8494-DC35E84786C2}"/>
-    <hyperlink ref="C10" r:id="rId6" display="https://www.amplifiedparts.com/products/washer-fiber-shoulder" xr:uid="{6CA84D7F-4D3A-D54C-965B-45E57A373BBC}"/>
-    <hyperlink ref="C11" r:id="rId7" display="https://www.amplifiedparts.com/products/potentiometer-alpha-linear-38-bushing" xr:uid="{4DD773A8-D00D-7644-9ECD-EC30584AFFAA}"/>
-    <hyperlink ref="C12" r:id="rId8" display="https://www.amplifiedparts.com/products/potentiometer-alpha-audio-38-bushing" xr:uid="{31178A28-70D0-C842-A2AD-A8A058D9D3DD}"/>
-    <hyperlink ref="C13" r:id="rId9" display="https://www.amplifiedparts.com/products/potentiometer-alpha-audio-38-bushing" xr:uid="{EA66D933-4D59-954C-BAD1-5FEE86CDFC97}"/>
-    <hyperlink ref="C14" r:id="rId10" display="https://www.amplifiedparts.com/products/mounting-plate-metal-1375-can-capacitor" xr:uid="{25BDDED4-FFD7-8F4F-88F4-A5297F81ADD4}"/>
-    <hyperlink ref="C15" r:id="rId11" display="https://www.amplifiedparts.com/products/cable-rca-right-angle-plugs" xr:uid="{10228D68-D86E-8940-B7D1-EC02355A2D60}"/>
-    <hyperlink ref="C16" r:id="rId12" display="https://www.amplifiedparts.com/products/capacitor-silver-mica-500v" xr:uid="{1763BE84-367A-6D43-9C10-DC9A3677F90B}"/>
-    <hyperlink ref="C17" r:id="rId13" display="https://www.amplifiedparts.com/products/capacitors-orange-drop-600v-polyester" xr:uid="{41A3A37F-DEF0-7141-9440-90A5FF2D04F4}"/>
-    <hyperlink ref="C18" r:id="rId14" display="https://www.amplifiedparts.com/products/capacitors-orange-drop-600v-polyester" xr:uid="{00CB709C-2061-7E4B-89AE-760FC7711CD3}"/>
-    <hyperlink ref="C19" r:id="rId15" display="https://www.amplifiedparts.com/products/capacitors-orange-drop-600v-polyester" xr:uid="{457CEA29-B9C0-CE46-823F-0B3F023F1B52}"/>
-    <hyperlink ref="C20" r:id="rId16" display="https://www.amplifiedparts.com/products/capacitors-orange-drop-600v-polyester" xr:uid="{03A0A83A-7377-CD4A-9C1E-DDE8806C7D7A}"/>
-    <hyperlink ref="C22" r:id="rId17" display="https://www.amplifiedparts.com/products/capacitors-orange-drop-600v-polyester" xr:uid="{B3764572-46E9-1043-8EDD-142A6FB43514}"/>
-    <hyperlink ref="C24" r:id="rId18" display="https://www.amplifiedparts.com/products/capacitor-ft-350v-100-f-axial-lead-electrolytic" xr:uid="{9B527B95-4CE9-F742-B365-5E62D1D2F34B}"/>
-    <hyperlink ref="C25" r:id="rId19" display="https://www.amplifiedparts.com/products/capacitor-ft-500v-axial-lead" xr:uid="{593D4072-FB31-ED4F-8347-E13364BA4376}"/>
-    <hyperlink ref="C26" r:id="rId20" display="https://www.amplifiedparts.com/products/capacitor-ft-500v-axial-lead" xr:uid="{CE79DD40-03E6-9944-A399-D5CB419B3264}"/>
-    <hyperlink ref="C27" r:id="rId21" xr:uid="{8B4F970B-85D0-CF47-9E17-E3DB4AB82C3B}"/>
-    <hyperlink ref="C28" r:id="rId22" display="https://www.amplifiedparts.com/products/socket-belton-micalex-8-pin-octal-mip" xr:uid="{B1955EDB-2B2F-2C46-89A2-73EA83B99AF8}"/>
-    <hyperlink ref="C29" r:id="rId23" display="https://www.amplifiedparts.com/products/switch-carling-toggle-spst-side-solder-lugs" xr:uid="{7D835C30-39A1-E14D-B210-56F45F93AAC0}"/>
-    <hyperlink ref="C38" r:id="rId24" xr:uid="{446A4929-572B-DE45-B933-EED363FE6136}"/>
-    <hyperlink ref="C31" r:id="rId25" display="https://www.amplifiedparts.com/products/jack-switchcraft-14-mono-2-conductor-shunt-tip" xr:uid="{20437A57-6CEF-2F46-AE02-1F24DD2D8942}"/>
-    <hyperlink ref="C32" r:id="rId26" display="https://www.amplifiedparts.com/products/tip-jack-insulated-deluxe" xr:uid="{994D40CA-AA99-434D-9E13-3BAAAF1E8109}"/>
-    <hyperlink ref="C33" r:id="rId27" display="https://www.amplifiedparts.com/products/rca-jack-switchcraft-rear-panel-mount-natural-insulator" xr:uid="{3C5DD7D3-79FD-7D41-8230-4E19EF7867AF}"/>
-    <hyperlink ref="C34" r:id="rId28" display="https://www.amplifiedparts.com/products/capacitor-ce-mfg-475v-20202020-f-electrolytic" xr:uid="{BBBB5C0A-336E-FF47-9F53-695CC4A1E87D}"/>
-    <hyperlink ref="C35" r:id="rId29" display="https://www.amplifiedparts.com/products/nut-kep-zinc-package-10" xr:uid="{683533DF-088F-7241-B0A7-6C5D32EB2FFA}"/>
-    <hyperlink ref="C36" r:id="rId30" display="https://www.amplifiedparts.com/products/screw-632-phillips-pan-head-machine-zinc" xr:uid="{32B4282D-6917-DA45-90A2-B056DB0EDF69}"/>
-    <hyperlink ref="C37" r:id="rId31" display="https://www.amplifiedparts.com/products/screw-632-phillips-pan-head-machine-zinc" xr:uid="{3ECEA5B5-DB19-BB4F-AC85-C6C9A79966C1}"/>
-    <hyperlink ref="C39" r:id="rId32" display="https://www.amplifiedparts.com/products/capacitor-600v-716p-series-polypropylene" xr:uid="{01626727-D59A-AE45-904D-5DEC75010C93}"/>
-    <hyperlink ref="C40" r:id="rId33" display="https://www.amplifiedparts.com/products/capacitor-630v-polypropylene-radial-leads" xr:uid="{4EBB18AD-6100-884D-9D78-7A16607C118D}"/>
-    <hyperlink ref="C42" r:id="rId34" xr:uid="{97E71238-E0D9-ED41-9FD4-55881FCCF1AE}"/>
-    <hyperlink ref="C43" r:id="rId35" display="https://www.amplifiedparts.com/products/chassis-box-hammond-unpainted-aluminum-437-x-237-x-122" xr:uid="{31888DCA-4426-444B-974A-E6526716EDE8}"/>
-    <hyperlink ref="C44" r:id="rId36" display="https://www.amplifiedparts.com/products/knob-chicken-head-raised" xr:uid="{B52594DC-6909-744D-BA87-2F3FD68B4AB0}"/>
-    <hyperlink ref="C46" r:id="rId37" display="https://www.amplifiedparts.com/products/capacitor-630v-polypropylene-radial-leads" xr:uid="{380C44B3-A3EB-2749-A694-BF348911BD2C}"/>
-    <hyperlink ref="C47" r:id="rId38" display="https://www.amplifiedparts.com/products/washer-internal-tooth-lock-zinc" xr:uid="{CB280860-5B31-6B41-8429-926A58467AD1}"/>
-    <hyperlink ref="C48" r:id="rId39" display="https://www.amplifiedparts.com/products/switch-rotary-3-poles-3-position" xr:uid="{5B95EB76-4FF1-6441-A991-5F4A5418B58E}"/>
-    <hyperlink ref="C49" r:id="rId40" display="https://www.amplifiedparts.com/products/washer-internal-tooth-lock-zinc" xr:uid="{44407C4A-3B71-0842-826A-41E11485AA86}"/>
-    <hyperlink ref="C50" r:id="rId41" display="https://www.amplifiedparts.com/products/standoff-6-32-female-aluminum" xr:uid="{EC4736A9-C917-C843-AF22-752E5FEB23DC}"/>
-    <hyperlink ref="C55" r:id="rId42" display="https://www.amplifiedparts.com/products/vacuum-tube-5751-tube-amp-doctor-premium-selected" xr:uid="{4912950B-C7F1-1948-82EA-45DE26B3F712}"/>
-    <hyperlink ref="C56" r:id="rId43" display="https://www.amplifiedparts.com/products/vacuum-tube-7025-tube-amp-doctor-high-grade" xr:uid="{9BD8E76F-19D2-3843-B818-7B8EB02F1E31}"/>
-    <hyperlink ref="C57" r:id="rId44" display="https://www.amplifiedparts.com/products/vacuum-tube-6l6wgc-tube-amp-doctor" xr:uid="{98CAA186-DA25-FC44-820D-1F20A7DE47BB}"/>
-    <hyperlink ref="C7" r:id="rId45" display="https://www.amplifiedparts.com/products/fuse-holder-3ag-type-high-quality" xr:uid="{152E0919-5501-DD44-95CF-91F92084A16B}"/>
-    <hyperlink ref="C21" r:id="rId46" xr:uid="{F975B4D8-4C09-B443-9FBA-C3A6C48B5B5C}"/>
-    <hyperlink ref="C45" r:id="rId47" xr:uid="{0C0C438D-27B3-A945-A47E-8EFD7A88A0E2}"/>
-    <hyperlink ref="C41" r:id="rId48" display="https://www.amplifiedparts.com/products/resistors-1w-carbon-film" xr:uid="{9EC41C18-4327-474C-820F-B7E6615117FC}"/>
-    <hyperlink ref="C30" r:id="rId49" xr:uid="{74390CCA-3976-FC41-BEFA-1A0070E273FC}"/>
-    <hyperlink ref="C54" r:id="rId50" xr:uid="{576CB110-0419-F842-9990-42E7EF931735}"/>
-    <hyperlink ref="G54" r:id="rId51" xr:uid="{E69CCDBC-6C40-DE46-BE3C-C4069BCEDB2F}"/>
-    <hyperlink ref="C51" r:id="rId52" xr:uid="{F2F617BC-7D75-CF42-B736-8614C283D61A}"/>
-    <hyperlink ref="G51" r:id="rId53" xr:uid="{D9CC8D2A-00E2-894C-8C57-434FE72FCBE4}"/>
-    <hyperlink ref="C53" r:id="rId54" xr:uid="{797AAEEA-9771-CB40-8715-81A1A41EDACA}"/>
-    <hyperlink ref="C52" r:id="rId55" xr:uid="{6D7EB390-EF0E-1942-A14E-C2A799B0578B}"/>
-    <hyperlink ref="G53" r:id="rId56" xr:uid="{44647F9C-7547-6E4C-B8A6-612CEE2F83BD}"/>
+    <hyperlink ref="C9" r:id="rId4" display="https://www.amplifiedparts.com/products/fuse-slo-blo-025-x-125" xr:uid="{62FD5CAC-91EB-0341-8494-DC35E84786C2}"/>
+    <hyperlink ref="C10" r:id="rId5" display="https://www.amplifiedparts.com/products/washer-fiber-shoulder" xr:uid="{6CA84D7F-4D3A-D54C-965B-45E57A373BBC}"/>
+    <hyperlink ref="C11" r:id="rId6" display="https://www.amplifiedparts.com/products/potentiometer-alpha-linear-38-bushing" xr:uid="{4DD773A8-D00D-7644-9ECD-EC30584AFFAA}"/>
+    <hyperlink ref="C12" r:id="rId7" display="https://www.amplifiedparts.com/products/potentiometer-alpha-audio-38-bushing" xr:uid="{31178A28-70D0-C842-A2AD-A8A058D9D3DD}"/>
+    <hyperlink ref="C13" r:id="rId8" display="https://www.amplifiedparts.com/products/potentiometer-alpha-audio-38-bushing" xr:uid="{EA66D933-4D59-954C-BAD1-5FEE86CDFC97}"/>
+    <hyperlink ref="C14" r:id="rId9" display="https://www.amplifiedparts.com/products/mounting-plate-metal-1375-can-capacitor" xr:uid="{25BDDED4-FFD7-8F4F-88F4-A5297F81ADD4}"/>
+    <hyperlink ref="C15" r:id="rId10" display="https://www.amplifiedparts.com/products/cable-rca-right-angle-plugs" xr:uid="{10228D68-D86E-8940-B7D1-EC02355A2D60}"/>
+    <hyperlink ref="C16" r:id="rId11" display="https://www.amplifiedparts.com/products/capacitor-silver-mica-500v" xr:uid="{1763BE84-367A-6D43-9C10-DC9A3677F90B}"/>
+    <hyperlink ref="C17" r:id="rId12" display="https://www.amplifiedparts.com/products/capacitors-orange-drop-600v-polyester" xr:uid="{41A3A37F-DEF0-7141-9440-90A5FF2D04F4}"/>
+    <hyperlink ref="C18" r:id="rId13" display="https://www.amplifiedparts.com/products/capacitors-orange-drop-600v-polyester" xr:uid="{00CB709C-2061-7E4B-89AE-760FC7711CD3}"/>
+    <hyperlink ref="C19" r:id="rId14" display="https://www.amplifiedparts.com/products/capacitors-orange-drop-600v-polyester" xr:uid="{457CEA29-B9C0-CE46-823F-0B3F023F1B52}"/>
+    <hyperlink ref="C20" r:id="rId15" display="https://www.amplifiedparts.com/products/capacitors-orange-drop-600v-polyester" xr:uid="{03A0A83A-7377-CD4A-9C1E-DDE8806C7D7A}"/>
+    <hyperlink ref="C22" r:id="rId16" display="https://www.amplifiedparts.com/products/capacitors-orange-drop-600v-polyester" xr:uid="{B3764572-46E9-1043-8EDD-142A6FB43514}"/>
+    <hyperlink ref="C24" r:id="rId17" display="https://www.amplifiedparts.com/products/capacitor-ft-350v-100-f-axial-lead-electrolytic" xr:uid="{9B527B95-4CE9-F742-B365-5E62D1D2F34B}"/>
+    <hyperlink ref="C25" r:id="rId18" display="https://www.amplifiedparts.com/products/capacitor-ft-500v-axial-lead" xr:uid="{593D4072-FB31-ED4F-8347-E13364BA4376}"/>
+    <hyperlink ref="C26" r:id="rId19" display="https://www.amplifiedparts.com/products/capacitor-ft-500v-axial-lead" xr:uid="{CE79DD40-03E6-9944-A399-D5CB419B3264}"/>
+    <hyperlink ref="C27" r:id="rId20" xr:uid="{8B4F970B-85D0-CF47-9E17-E3DB4AB82C3B}"/>
+    <hyperlink ref="C28" r:id="rId21" display="https://www.amplifiedparts.com/products/socket-belton-micalex-8-pin-octal-mip" xr:uid="{B1955EDB-2B2F-2C46-89A2-73EA83B99AF8}"/>
+    <hyperlink ref="C29" r:id="rId22" display="https://www.amplifiedparts.com/products/switch-carling-toggle-spst-side-solder-lugs" xr:uid="{7D835C30-39A1-E14D-B210-56F45F93AAC0}"/>
+    <hyperlink ref="C38" r:id="rId23" xr:uid="{446A4929-572B-DE45-B933-EED363FE6136}"/>
+    <hyperlink ref="C31" r:id="rId24" display="https://www.amplifiedparts.com/products/jack-switchcraft-14-mono-2-conductor-shunt-tip" xr:uid="{20437A57-6CEF-2F46-AE02-1F24DD2D8942}"/>
+    <hyperlink ref="C32" r:id="rId25" display="https://www.amplifiedparts.com/products/tip-jack-insulated-deluxe" xr:uid="{994D40CA-AA99-434D-9E13-3BAAAF1E8109}"/>
+    <hyperlink ref="C33" r:id="rId26" display="https://www.amplifiedparts.com/products/rca-jack-switchcraft-rear-panel-mount-natural-insulator" xr:uid="{3C5DD7D3-79FD-7D41-8230-4E19EF7867AF}"/>
+    <hyperlink ref="C34" r:id="rId27" display="https://www.amplifiedparts.com/products/capacitor-ce-mfg-475v-20202020-f-electrolytic" xr:uid="{BBBB5C0A-336E-FF47-9F53-695CC4A1E87D}"/>
+    <hyperlink ref="C35" r:id="rId28" display="https://www.amplifiedparts.com/products/nut-kep-zinc-package-10" xr:uid="{683533DF-088F-7241-B0A7-6C5D32EB2FFA}"/>
+    <hyperlink ref="C36" r:id="rId29" display="https://www.amplifiedparts.com/products/screw-632-phillips-pan-head-machine-zinc" xr:uid="{32B4282D-6917-DA45-90A2-B056DB0EDF69}"/>
+    <hyperlink ref="C37" r:id="rId30" display="https://www.amplifiedparts.com/products/screw-632-phillips-pan-head-machine-zinc" xr:uid="{3ECEA5B5-DB19-BB4F-AC85-C6C9A79966C1}"/>
+    <hyperlink ref="C39" r:id="rId31" display="https://www.amplifiedparts.com/products/capacitor-600v-716p-series-polypropylene" xr:uid="{01626727-D59A-AE45-904D-5DEC75010C93}"/>
+    <hyperlink ref="C40" r:id="rId32" display="https://www.amplifiedparts.com/products/capacitor-630v-polypropylene-radial-leads" xr:uid="{4EBB18AD-6100-884D-9D78-7A16607C118D}"/>
+    <hyperlink ref="C42" r:id="rId33" xr:uid="{97E71238-E0D9-ED41-9FD4-55881FCCF1AE}"/>
+    <hyperlink ref="C43" r:id="rId34" display="https://www.amplifiedparts.com/products/chassis-box-hammond-unpainted-aluminum-437-x-237-x-122" xr:uid="{31888DCA-4426-444B-974A-E6526716EDE8}"/>
+    <hyperlink ref="C44" r:id="rId35" display="https://www.amplifiedparts.com/products/knob-chicken-head-raised" xr:uid="{B52594DC-6909-744D-BA87-2F3FD68B4AB0}"/>
+    <hyperlink ref="C46" r:id="rId36" display="https://www.amplifiedparts.com/products/capacitor-630v-polypropylene-radial-leads" xr:uid="{380C44B3-A3EB-2749-A694-BF348911BD2C}"/>
+    <hyperlink ref="C47" r:id="rId37" display="https://www.amplifiedparts.com/products/washer-internal-tooth-lock-zinc" xr:uid="{CB280860-5B31-6B41-8429-926A58467AD1}"/>
+    <hyperlink ref="C48" r:id="rId38" display="https://www.amplifiedparts.com/products/switch-rotary-3-poles-3-position" xr:uid="{5B95EB76-4FF1-6441-A991-5F4A5418B58E}"/>
+    <hyperlink ref="C49" r:id="rId39" display="https://www.amplifiedparts.com/products/washer-internal-tooth-lock-zinc" xr:uid="{44407C4A-3B71-0842-826A-41E11485AA86}"/>
+    <hyperlink ref="C50" r:id="rId40" display="https://www.amplifiedparts.com/products/standoff-6-32-female-aluminum" xr:uid="{EC4736A9-C917-C843-AF22-752E5FEB23DC}"/>
+    <hyperlink ref="C55" r:id="rId41" display="https://www.amplifiedparts.com/products/vacuum-tube-5751-tube-amp-doctor-premium-selected" xr:uid="{4912950B-C7F1-1948-82EA-45DE26B3F712}"/>
+    <hyperlink ref="C56" r:id="rId42" display="https://www.amplifiedparts.com/products/vacuum-tube-7025-tube-amp-doctor-high-grade" xr:uid="{9BD8E76F-19D2-3843-B818-7B8EB02F1E31}"/>
+    <hyperlink ref="C57" r:id="rId43" display="https://www.amplifiedparts.com/products/vacuum-tube-6l6wgc-tube-amp-doctor" xr:uid="{98CAA186-DA25-FC44-820D-1F20A7DE47BB}"/>
+    <hyperlink ref="C7" r:id="rId44" display="https://www.amplifiedparts.com/products/fuse-holder-3ag-type-high-quality" xr:uid="{152E0919-5501-DD44-95CF-91F92084A16B}"/>
+    <hyperlink ref="C21" r:id="rId45" xr:uid="{F975B4D8-4C09-B443-9FBA-C3A6C48B5B5C}"/>
+    <hyperlink ref="C45" r:id="rId46" xr:uid="{0C0C438D-27B3-A945-A47E-8EFD7A88A0E2}"/>
+    <hyperlink ref="C41" r:id="rId47" display="https://www.amplifiedparts.com/products/resistors-1w-carbon-film" xr:uid="{9EC41C18-4327-474C-820F-B7E6615117FC}"/>
+    <hyperlink ref="C30" r:id="rId48" xr:uid="{74390CCA-3976-FC41-BEFA-1A0070E273FC}"/>
+    <hyperlink ref="C54" r:id="rId49" xr:uid="{576CB110-0419-F842-9990-42E7EF931735}"/>
+    <hyperlink ref="G54" r:id="rId50" xr:uid="{E69CCDBC-6C40-DE46-BE3C-C4069BCEDB2F}"/>
+    <hyperlink ref="C51" r:id="rId51" xr:uid="{F2F617BC-7D75-CF42-B736-8614C283D61A}"/>
+    <hyperlink ref="G51" r:id="rId52" xr:uid="{D9CC8D2A-00E2-894C-8C57-434FE72FCBE4}"/>
+    <hyperlink ref="C53" r:id="rId53" xr:uid="{797AAEEA-9771-CB40-8715-81A1A41EDACA}"/>
+    <hyperlink ref="C52" r:id="rId54" xr:uid="{6D7EB390-EF0E-1942-A14E-C2A799B0578B}"/>
+    <hyperlink ref="G53" r:id="rId55" xr:uid="{44647F9C-7547-6E4C-B8A6-612CEE2F83BD}"/>
+    <hyperlink ref="C8" r:id="rId56" display="https://www.amplifiedparts.com/products/fuse-slo-blo-025-x-125" xr:uid="{CB55DA37-E898-DD4C-A111-82ED00860EB5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>